<commit_message>
feat: sms dashboard & sms manual
</commit_message>
<xml_diff>
--- a/api/service/EXPORT_TEMPLATE.xlsx
+++ b/api/service/EXPORT_TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P-BANK\GIT\hopeful\api\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C0B050-CA64-4CB0-9DBB-DE8538127542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA95361A-A0A1-47FE-9CAB-4773EAB484F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{0B2911A3-578A-4BC6-BAEF-48521B2BC841}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B2911A3-578A-4BC6-BAEF-48521B2BC841}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>วันที่ทำรายการ</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>คนดูแล nickname</t>
+  </si>
+  <si>
+    <t>Tracking</t>
+  </si>
+  <si>
+    <t>ขนส่ง</t>
   </si>
 </sst>
 </file>
@@ -564,11 +570,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFB181E-5A94-4E63-BF94-5FECEFD59A42}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -595,12 +599,12 @@
     <col min="23" max="23" width="10.5546875" style="6" customWidth="1"/>
     <col min="24" max="24" width="11.21875" style="8" customWidth="1"/>
     <col min="25" max="25" width="12.5546875" style="6" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" style="6"/>
-    <col min="27" max="27" width="17.88671875" style="6" customWidth="1"/>
-    <col min="28" max="28" width="15.6640625" customWidth="1"/>
+    <col min="26" max="28" width="8.77734375" style="6"/>
+    <col min="29" max="29" width="17.88671875" style="6" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -680,13 +684,19 @@
         <v>21</v>
       </c>
       <c r="AA1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="14"/>

</xml_diff>

<commit_message>
feat: Menu create product group
</commit_message>
<xml_diff>
--- a/api/service/EXPORT_TEMPLATE.xlsx
+++ b/api/service/EXPORT_TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P-BANK\GIT\hopeful\api\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA95361A-A0A1-47FE-9CAB-4773EAB484F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C0B050-CA64-4CB0-9DBB-DE8538127542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B2911A3-578A-4BC6-BAEF-48521B2BC841}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{0B2911A3-578A-4BC6-BAEF-48521B2BC841}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>วันที่ทำรายการ</t>
   </si>
@@ -116,12 +116,6 @@
   </si>
   <si>
     <t>คนดูแล nickname</t>
-  </si>
-  <si>
-    <t>Tracking</t>
-  </si>
-  <si>
-    <t>ขนส่ง</t>
   </si>
 </sst>
 </file>
@@ -570,9 +564,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFB181E-5A94-4E63-BF94-5FECEFD59A42}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -599,12 +595,12 @@
     <col min="23" max="23" width="10.5546875" style="6" customWidth="1"/>
     <col min="24" max="24" width="11.21875" style="8" customWidth="1"/>
     <col min="25" max="25" width="12.5546875" style="6" customWidth="1"/>
-    <col min="26" max="28" width="8.77734375" style="6"/>
-    <col min="29" max="29" width="17.88671875" style="6" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" customWidth="1"/>
+    <col min="26" max="26" width="8.77734375" style="6"/>
+    <col min="27" max="27" width="17.88671875" style="6" customWidth="1"/>
+    <col min="28" max="28" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -684,19 +680,13 @@
         <v>21</v>
       </c>
       <c r="AA1" s="16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD1" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="14"/>

</xml_diff>